<commit_message>
Changes to date tracker
</commit_message>
<xml_diff>
--- a/Date tracker Gantt chart.xlsx
+++ b/Date tracker Gantt chart.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6E7E35DF-7658-45FE-8220-E44ECE8EAC22}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9675" activeTab="1" xr2:uid="{568C94E4-E3F7-4EB4-8281-4914A18C47B4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Chart Data" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <definedName name="Start_Date">IFERROR(IF(MIN(Tasks[Start Date])="",TODAY(),MIN(Tasks[Start Date])),"")</definedName>
     <definedName name="Track_Today">'Chart Data'!$D$2</definedName>
   </definedNames>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -328,16 +327,16 @@
     <t>Create TDD</t>
   </si>
   <si>
-    <t>Character can move</t>
-  </si>
-  <si>
     <t>Create inventory item and in-world item</t>
+  </si>
+  <si>
+    <t>Movement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -517,7 +516,7 @@
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Comma [0]" xfId="7" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Date" xfId="6" xr:uid="{6EB70F65-3733-4804-9FF5-428A9E5C4ABE}"/>
+    <cellStyle name="Date" xfId="6"/>
     <cellStyle name="Explanatory Text" xfId="5" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
@@ -605,7 +604,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -631,7 +629,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -660,7 +657,6 @@
         <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -724,7 +720,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Date Tracking Gantt Chart" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Date Tracking Gantt Chart" pivot="0" count="5" xr9:uid="{FE5A7A51-290B-4843-B986-5E08FCB37B0E}">
+    <tableStyle name="Date Tracking Gantt Chart" pivot="0" count="5">
       <tableStyleElement type="wholeTable" dxfId="22"/>
       <tableStyleElement type="headerRow" dxfId="21"/>
       <tableStyleElement type="firstColumn" dxfId="20"/>
@@ -787,12 +783,13 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EBAB2AEA-EC22-49EC-A886-CED5D5C08929}" type="CELLRANGE">
+                    <a:fld id="{28B28128-A27F-418B-B4C4-5CE0AB204E5A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -810,6 +807,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -821,12 +819,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F481F707-0761-4E0B-A6A6-9C9D32C5B1A6}" type="CELLRANGE">
+                    <a:fld id="{CEC678F7-2914-480B-B408-DB2266662EB8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -844,6 +843,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -855,12 +855,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{90F5C704-CF37-407A-9068-682F6F4E5F59}" type="CELLRANGE">
+                    <a:fld id="{D004312A-4524-422D-8724-535B945A03CE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -878,6 +879,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -889,12 +891,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A218DF00-3A4A-491C-B7CE-511B9F6CD742}" type="CELLRANGE">
+                    <a:fld id="{C43F7448-D1D1-4759-A4C1-82BD2CC1D959}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -912,6 +915,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -923,12 +927,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{40551370-F6E7-4E8A-8A91-BDCB5C9ABB30}" type="CELLRANGE">
+                    <a:fld id="{DAABF432-223C-4918-AA3F-EC9D4D405C4B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -946,6 +951,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -957,12 +963,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D222167A-1D6E-4067-ADC8-50C5CE3CC304}" type="CELLRANGE">
+                    <a:fld id="{F33BF101-597C-4D20-8E06-A72540A092CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -980,6 +987,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -991,12 +999,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B7BA8C1-A4EF-486A-B07E-518EEEB288FA}" type="CELLRANGE">
+                    <a:fld id="{A68F0C7D-5590-413D-83BE-2C59018499EB}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1014,6 +1023,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1062,6 +1072,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1079,25 +1090,25 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>4</c:v>
+                    <c:v>8</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5</c:v>
+                    <c:v>7</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>10</c:v>
+                    <c:v>15</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6</c:v>
+                    <c:v>15</c:v>
                   </c:pt>
                   <c:pt idx="4">
                     <c:v>3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>15</c:v>
+                    <c:v>9</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>15</c:v>
+                    <c:v>0</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1132,25 +1143,25 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>43387</c:v>
+                  <c:v>43397</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43388</c:v>
+                  <c:v>43400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43390</c:v>
+                  <c:v>43406</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43397</c:v>
+                  <c:v>43413</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43400</c:v>
+                  <c:v>43430</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43406</c:v>
+                  <c:v>43432</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43413</c:v>
+                  <c:v>43432</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1180,7 +1191,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1193,25 +1204,22 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="7"/>
                   <c:pt idx="0">
-                    <c:v>Edit and Review SRS</c:v>
+                    <c:v>Create TDD</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Create Vision Document</c:v>
+                    <c:v>Character Movement</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>Create GDD</c:v>
+                    <c:v>Create a modular item system</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Create TDD</c:v>
+                    <c:v>Create modular item interactions</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Character can move</c:v>
+                    <c:v>Create inventory item and in-world item</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>Create a modular item system</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>Create modular item interactions</c:v>
+                    <c:v>Bug Fixes</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -1229,9 +1237,6 @@
               <c:f>'Dynamic Chart Data Hidden'!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Today</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
@@ -1256,6 +1261,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
@@ -1273,7 +1279,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{98086980-2079-433A-A231-CBD37107C645}" type="CELLRANGE">
+                    <a:fld id="{0F680057-D108-4FBE-B534-778DD3F15102}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1100">
@@ -1323,6 +1329,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1333,6 +1340,7 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
@@ -1350,7 +1358,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000015-CCF3-4D6B-A363-E3E4CAC6EE6E}"/>
                 </c:ext>
@@ -1425,10 +1435,10 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>43388</c:v>
+                  <c:v>43397</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43388</c:v>
+                  <c:v>43397</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1440,10 +1450,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1455,9 +1465,6 @@
                 <c15:f>'Dynamic Chart Data Hidden'!$B$2</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="1"/>
-                  <c:pt idx="0">
-                    <c:v>Today</c:v>
-                  </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
             </c:ext>
@@ -1492,12 +1499,13 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E0A60139-BD2A-4367-B58F-A06110C31B97}" type="CELLRANGE">
+                    <a:fld id="{6F423A9F-5A3A-4FD0-AC09-2955AE5B3FED}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1515,6 +1523,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1525,12 +1534,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{52E7CFB3-5A6D-4181-933C-A056779B55B4}" type="CELLRANGE">
+                    <a:fld id="{06052A70-B7FD-4FF9-AC44-2CEE7B6F89BE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1548,6 +1558,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1559,12 +1570,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2691DCB-F310-4C45-B6F5-539515308D22}" type="CELLRANGE">
+                    <a:fld id="{E7E9996D-12CE-41C7-B4A6-2D2A57AADFD8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1582,6 +1594,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1593,12 +1606,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="3"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3BE739E6-E0FB-4574-8C27-F660F32DFEC7}" type="CELLRANGE">
+                    <a:fld id="{D58CA157-5A7A-48D4-ABB4-E2B99EA09E78}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1616,6 +1630,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1627,12 +1642,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DE3909C-A02C-484F-888E-6AD023C5EC95}" type="CELLRANGE">
+                    <a:fld id="{7E0B657F-0758-4C62-BED1-6470D6C4A98F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1650,6 +1666,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1661,12 +1678,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{278D01F2-B3EE-4997-B945-0DAA51034DC2}" type="CELLRANGE">
+                    <a:fld id="{93139537-89E8-4D34-B66C-472BBF09CF36}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1684,6 +1702,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1695,12 +1714,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4F6C88B2-91A0-4093-9FEF-B9571E0FDB1E}" type="CELLRANGE">
+                    <a:fld id="{238C5C31-E2E1-422D-9F31-72AFAFD23838}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1718,6 +1738,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1729,12 +1750,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{482CE2FA-F968-4C8B-8783-6E9B0509CC88}" type="CELLRANGE">
+                    <a:fld id="{1D4B3E20-872A-4476-987A-EEB4374A126B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1752,6 +1774,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1763,12 +1786,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{207BCD03-3552-4D02-AD92-5EBBEF8D36DC}" type="CELLRANGE">
+                    <a:fld id="{BA865317-D096-47BA-82E3-32C4AD2357C5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1786,6 +1810,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1797,12 +1822,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C459193D-AFB8-4B98-B575-8D67BDDF6805}" type="CELLRANGE">
+                    <a:fld id="{02A141C4-092B-4659-8F28-49957C720392}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1820,6 +1846,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1831,12 +1858,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{28D306EC-0303-44A7-9B73-53A5E8917C7D}" type="CELLRANGE">
+                    <a:fld id="{D392C6A6-1937-4BD8-A9E7-977331618E93}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1854,6 +1882,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1865,12 +1894,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F5C8CD22-8EC6-412F-BB4E-9BE3F9BA234F}" type="CELLRANGE">
+                    <a:fld id="{F8DC4173-5909-4284-A1C4-FF169C14EE92}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1888,6 +1918,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1899,12 +1930,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="12"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{895CD933-A1FC-4A77-8345-F271BCADEAB3}" type="CELLRANGE">
+                    <a:fld id="{DE507C2B-8499-48CF-AE9B-BABFE1BC63FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1922,6 +1954,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1933,12 +1966,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="13"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{854E5A85-3583-47C7-A8AE-9AC5C3171B23}" type="CELLRANGE">
+                    <a:fld id="{7D695CC5-51B2-4C4C-AA27-9AA7889E16E1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1956,6 +1990,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -1967,12 +2002,13 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="14"/>
+              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8F0985A-13D9-4DB8-96E9-4AF0E9C27DE3}" type="CELLRANGE">
+                    <a:fld id="{247BE516-0468-4F44-8256-5CC1BCF2912E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1990,6 +2026,7 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -2060,6 +2097,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2081,40 +2119,40 @@
                   <c:v>43399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43402</c:v>
+                  <c:v>43404</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43402</c:v>
+                  <c:v>43407</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43402</c:v>
+                  <c:v>43427</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43402</c:v>
+                  <c:v>43440</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43402</c:v>
+                  <c:v>43440</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>43402</c:v>
+                  <c:v>43440</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43402</c:v>
+                  <c:v>43440</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43402</c:v>
+                  <c:v>43440</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>43402</c:v>
+                  <c:v>43440</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>43402</c:v>
+                  <c:v>43440</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>43402</c:v>
+                  <c:v>43440</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>43402</c:v>
+                  <c:v>43440</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2132,19 +2170,19 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -2188,6 +2226,18 @@
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>GDD</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>TDD</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Movement</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Item System</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>MVP</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -2288,6 +2338,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2295,7 +2346,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2882,7 +2932,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="'Dynamic Chart Data Hidden'!$B$8" horiz="1" max="100" page="4" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="'Dynamic Chart Data Hidden'!$B$8" horiz="1" max="100" page="4" val="3"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2932,7 +2982,7 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>38100</xdr:colOff>
           <xdr:row>0</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>88900</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>17</xdr:col>
@@ -2979,17 +3029,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02DCCC90-6A03-4F39-A9BB-582A9958C0EF}" name="Tasks" displayName="Tasks" ref="G5:K25" totalsRowShown="0">
-  <autoFilter ref="G5:K25" xr:uid="{22AFF5BD-21AE-4912-A8C2-DAA508F7F469}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tasks" displayName="Tasks" ref="G5:K25" totalsRowShown="0">
+  <autoFilter ref="G5:K25"/>
   <sortState ref="G6:J25">
     <sortCondition ref="H5:H25"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="4" xr3:uid="{8D50EF12-D72C-4368-8326-03E797ADB3CB}" name="No." dataDxfId="17"/>
-    <tableColumn id="1" xr3:uid="{6CD36057-C64E-48FF-8662-5FD7B4F32BF9}" name="Start Date" dataCellStyle="Date"/>
-    <tableColumn id="2" xr3:uid="{96A5962B-4C06-442F-8E89-23604EF5C723}" name="End Date" dataCellStyle="Date"/>
-    <tableColumn id="3" xr3:uid="{16FB4742-B3F6-42FC-9A10-1D5DD112F2D1}" name="Task"/>
-    <tableColumn id="5" xr3:uid="{D768AAFA-90E4-428E-833F-D632C9128159}" name="Duration in days" dataDxfId="16" dataCellStyle="Comma [0]">
+    <tableColumn id="4" name="No." dataDxfId="17"/>
+    <tableColumn id="1" name="Start Date" dataCellStyle="Date"/>
+    <tableColumn id="2" name="End Date" dataCellStyle="Date"/>
+    <tableColumn id="3" name="Task"/>
+    <tableColumn id="5" name="Duration in days" dataDxfId="16" dataCellStyle="Comma [0]">
       <calculatedColumnFormula>IFERROR(IF(LEN(Tasks[[#This Row],[Start Date]])=0,"",(INT(Tasks[[#This Row],[End Date]])-INT(Tasks[[#This Row],[Start Date]]))-(INT(Tasks[[#This Row],[Start Date]])-INT(Tasks[[#This Row],[Start Date]]))+1),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2998,8 +3048,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{53B1C454-C288-45B2-94F8-38A514974D6C}" name="Milestones" displayName="Milestones" ref="B5:E20" totalsRowShown="0">
-  <autoFilter ref="B5:E20" xr:uid="{E06B7BB2-84B0-4701-96A3-1920CD80CF06}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Milestones" displayName="Milestones" ref="B5:E20" totalsRowShown="0">
+  <autoFilter ref="B5:E20">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -3009,10 +3059,10 @@
     <sortCondition ref="D6:D16"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="5" xr3:uid="{114C9E6F-5647-4D28-B915-EB9BAEB0DA0B}" name="No." dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{2EB2227F-D85F-4004-8BC5-DEE0E8CC2A93}" name="Position" dataDxfId="14"/>
-    <tableColumn id="1" xr3:uid="{6E180707-6E70-48F0-B1D1-03AC999F6B82}" name="date" dataCellStyle="Date"/>
-    <tableColumn id="2" xr3:uid="{53D70D33-C6AC-47A5-B1DA-19C54C29A9FB}" name="Milestone"/>
+    <tableColumn id="5" name="No." dataDxfId="15"/>
+    <tableColumn id="3" name="Position" dataDxfId="14"/>
+    <tableColumn id="1" name="date" dataCellStyle="Date"/>
+    <tableColumn id="2" name="Milestone"/>
   </tableColumns>
   <tableStyleInfo name="Date Tracking Gantt Chart" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3024,24 +3074,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E532DFFE-02B7-4471-8985-080BC03A219D}" name="DynamicTaskData" displayName="DynamicTaskData" ref="B14:E21" totalsRowShown="0">
-  <autoFilter ref="B14:E21" xr:uid="{45ED1FBB-4F4C-4AC7-936B-6EAE70254C65}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="DynamicTaskData" displayName="DynamicTaskData" ref="B14:E21" totalsRowShown="0">
+  <autoFilter ref="B14:E21">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{74A625E2-A69E-4395-831A-7686CCC538CA}" name="Tasks" dataDxfId="12">
+    <tableColumn id="1" name="Tasks" dataDxfId="12">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Chart Data'!$H6,ScrollingIncrement[scroll increment],0,1,1))=0,"",IF(OR(OFFSET('Chart Data'!$I6,ScrollingIncrement[scroll increment],0,1,1)&lt;=$B$12,OFFSET('Chart Data'!$H6,ScrollingIncrement[scroll increment],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tasks[],OFFSET('Chart Data'!$G6,ScrollingIncrement[scroll increment],0,1,1),4),"")),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{67A68433-98C6-4D8B-B13E-5A174B091BFD}" name="Start date" dataDxfId="11" dataCellStyle="Date">
+    <tableColumn id="2" name="Start date" dataDxfId="11" dataCellStyle="Date">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,$B$11,INDEX(Tasks[],OFFSET('Chart Data'!$G6,ScrollingIncrement[scroll increment],0,1,1),2)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F8FBD7F0-C854-4F78-A244-B23F2FFF6E70}" name="Task duration in days" dataDxfId="10">
+    <tableColumn id="3" name="Task duration in days" dataDxfId="10">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,0,IF(AND('Chart Data'!$H6&lt;=$B$12,'Chart Data'!$I6&gt;=$B$12),ABS(OFFSET('Chart Data'!$H6,ScrollingIncrement[scroll increment],0,1,1)-$B$12)+1,OFFSET('Chart Data'!$K6,ScrollingIncrement[scroll increment],0,1,1))),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5A2DA5AB-D865-4B01-B889-2961800BAEFD}" name="position" dataDxfId="9">
+    <tableColumn id="4" name="position" dataDxfId="9">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,"",ROW($A1)),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3055,13 +3105,13 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{30441B7F-CD77-4D69-8E7E-DBBDDD14279F}" name="TodayHighlight" displayName="TodayHighlight" ref="B3:C5" totalsRowShown="0">
-  <autoFilter ref="B3:C5" xr:uid="{C74C9E73-4A4C-4834-9227-5225090C02B4}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="TodayHighlight" displayName="TodayHighlight" ref="B3:C5" totalsRowShown="0">
+  <autoFilter ref="B3:C5"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C38F7B9B-A971-4488-8015-29B0727A34E7}" name="today highlight x co-ord" dataDxfId="8">
+    <tableColumn id="1" name="today highlight x co-ord" dataDxfId="8">
       <calculatedColumnFormula>IFERROR(IF(TODAY()&lt;MIN(DynamicTaskData[Start date]),MIN($B$11,MIN(DynamicTaskData[Start date])),TODAY()),TODAY())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{0976B376-4D30-4099-AE10-A329AAD22F6E}" name="y co-ord" dataDxfId="7">
+    <tableColumn id="2" name="y co-ord" dataDxfId="7">
       <calculatedColumnFormula>IFERROR(IF(Track_Today="Yes",IF(TODAY()&lt;MIN(DynamicTaskData[Start date]),0,9),0),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3075,20 +3125,20 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{5FFCDDBD-CD08-4F0C-8197-655C2C936E7C}" name="DynamicMilestoneData" displayName="DynamicMilestoneData" ref="G17:I32" totalsRowShown="0">
-  <autoFilter ref="G17:I32" xr:uid="{36CE19C9-41B5-47A8-AAA1-A3D6AC913D8B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="DynamicMilestoneData" displayName="DynamicMilestoneData" ref="G17:I32" totalsRowShown="0">
+  <autoFilter ref="G17:I32">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{B32D10F3-8C97-4D87-8F09-C4C9DB7410B5}" name="Milestones" dataDxfId="6">
+    <tableColumn id="1" name="Milestones" dataDxfId="6">
       <calculatedColumnFormula>IFERROR(IF(LEN('Chart Data'!D6)=0,"",IF(AND('Chart Data'!D6&lt;=$B$12,'Chart Data'!D6&gt;=$B$11-$D$11),'Chart Data'!E6,"")),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{08699A2C-FE9E-454E-85A5-61493B3B2502}" name="Date" dataDxfId="5" dataCellStyle="Date">
+    <tableColumn id="4" name="Date" dataDxfId="5" dataCellStyle="Date">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D6),2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FF95A456-DC6C-4DEF-A422-1A60C8530445}" name="Baseline" dataDxfId="4">
+    <tableColumn id="5" name="Baseline" dataDxfId="4">
       <calculatedColumnFormula>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C6),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3097,12 +3147,12 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D6206301-033F-458C-8270-AB1B58CF736C}" name="ScrollingIncrement" displayName="ScrollingIncrement" ref="B7:B8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
-  <autoFilter ref="B7:B8" xr:uid="{EF98147B-BF9A-4D76-A56A-BD910CB7D4BE}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="ScrollingIncrement" displayName="ScrollingIncrement" ref="B7:B8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2">
+  <autoFilter ref="B7:B8">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{F9A5A7B8-7EE1-4D44-B78F-710AFC7920AA}" name="scroll increment" dataDxfId="1"/>
+    <tableColumn id="1" name="scroll increment" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="Date Tracking Gantt Chart" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -3114,10 +3164,10 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{4FA05E03-B076-4E71-A71C-74071F60185C}" name="chartingRange" displayName="chartingRange" ref="B10:B12" totalsRowShown="0">
-  <autoFilter ref="B10:B12" xr:uid="{DDE82E12-4FE9-46D1-8EAA-6B89FFED0A50}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="chartingRange" displayName="chartingRange" ref="B10:B12" totalsRowShown="0">
+  <autoFilter ref="B10:B12"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{1D49A440-6CFE-4E17-92DB-D396A59981B6}" name="Charting Range" dataDxfId="0">
+    <tableColumn id="1" name="Charting Range" dataDxfId="0">
       <calculatedColumnFormula>IFERROR(IF(LEN(#REF!)=0,End_Date+15,MIN(#REF!)+15),TODAY())</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3126,10 +3176,10 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{9823DB67-B8D9-46C5-923A-01532D552F07}" name="Ageoff" displayName="Ageoff" ref="D10:D11" totalsRowShown="0">
-  <autoFilter ref="D10:D11" xr:uid="{A497F6DC-1163-4C3D-B959-8F6736298A72}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Ageoff" displayName="Ageoff" ref="D10:D11" totalsRowShown="0">
+  <autoFilter ref="D10:D11"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{D9C67577-58B7-4BF1-9128-CF610F096B3F}" name="ageoff"/>
+    <tableColumn id="1" name="ageoff"/>
   </tableColumns>
   <tableStyleInfo name="Date Tracking Gantt Chart" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3431,32 +3481,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61AFF321-794A-47AE-98B5-6FA25ADFEE58}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView showGridLines="0" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="30.7109375" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" customWidth="1"/>
-    <col min="11" max="11" width="19.28515625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" customWidth="1"/>
+    <col min="5" max="5" width="30.7265625" customWidth="1"/>
+    <col min="6" max="6" width="2.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.7265625" customWidth="1"/>
+    <col min="8" max="8" width="12.7265625" customWidth="1"/>
+    <col min="9" max="9" width="14.7265625" customWidth="1"/>
+    <col min="10" max="10" width="30.7265625" customWidth="1"/>
+    <col min="11" max="11" width="19.26953125" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>28</v>
       </c>
@@ -3464,7 +3514,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>42</v>
       </c>
@@ -3476,7 +3526,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="35.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="35.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
         <v>44</v>
       </c>
@@ -3487,7 +3537,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="102.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="104.5" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>45</v>
       </c>
@@ -3519,7 +3569,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
         <v>46</v>
       </c>
@@ -3551,7 +3601,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="14"/>
       <c r="B6" s="11">
         <v>1</v>
@@ -3584,7 +3634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B7" s="11">
         <v>2</v>
       </c>
@@ -3614,12 +3664,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B8" s="11">
         <v>3</v>
       </c>
       <c r="C8" s="21">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D8" s="22">
         <v>43399</v>
@@ -3644,12 +3694,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B9" s="11">
         <v>4</v>
       </c>
       <c r="C9" s="21">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D9" s="22">
         <v>43404</v>
@@ -3674,18 +3724,18 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B10" s="11">
         <v>5</v>
       </c>
       <c r="C10" s="21">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D10" s="22">
-        <v>43406</v>
+        <v>43407</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="G10" s="11">
         <v>5</v>
@@ -3697,19 +3747,19 @@
         <v>43406</v>
       </c>
       <c r="J10" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K10" s="26">
         <f>IFERROR(IF(LEN(Tasks[[#This Row],[Start Date]])=0,"",(INT(Tasks[[#This Row],[End Date]])-INT(Tasks[[#This Row],[Start Date]]))-(INT(Tasks[[#This Row],[Start Date]])-INT(Tasks[[#This Row],[Start Date]]))+1),"")</f>
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B11" s="11">
         <v>6</v>
       </c>
       <c r="C11" s="21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D11" s="22">
         <v>43427</v>
@@ -3734,12 +3784,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B12" s="11">
         <v>7</v>
       </c>
       <c r="C12" s="21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D12" s="22">
         <v>43440</v>
@@ -3764,7 +3814,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="11"/>
       <c r="C13" s="21"/>
       <c r="D13" s="22"/>
@@ -3779,14 +3829,14 @@
         <v>43432</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K13" s="26">
         <f>IFERROR(IF(LEN(Tasks[[#This Row],[Start Date]])=0,"",(INT(Tasks[[#This Row],[End Date]])-INT(Tasks[[#This Row],[Start Date]]))-(INT(Tasks[[#This Row],[Start Date]])-INT(Tasks[[#This Row],[Start Date]]))+1),"")</f>
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B14" s="11"/>
       <c r="C14" s="21"/>
       <c r="D14" s="22"/>
@@ -3808,7 +3858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B15" s="11"/>
       <c r="C15" s="21"/>
       <c r="D15" s="22"/>
@@ -3822,7 +3872,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B16" s="11"/>
       <c r="C16" s="21"/>
       <c r="D16" s="22"/>
@@ -3836,7 +3886,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B17" s="11"/>
       <c r="C17" s="21"/>
       <c r="D17" s="22"/>
@@ -3850,7 +3900,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B18" s="11"/>
       <c r="C18" s="21"/>
       <c r="D18" s="22"/>
@@ -3864,7 +3914,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" s="11"/>
       <c r="C19" s="21"/>
       <c r="D19" s="22"/>
@@ -3878,7 +3928,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B20" s="11"/>
       <c r="C20" s="21"/>
       <c r="D20" s="22"/>
@@ -3892,7 +3942,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>48</v>
       </c>
@@ -3911,7 +3961,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G22" s="11"/>
       <c r="H22" s="22"/>
       <c r="I22" s="22"/>
@@ -3921,7 +3971,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G23" s="11"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
@@ -3931,7 +3981,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G24" s="11"/>
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
@@ -3941,7 +3991,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G25" s="11"/>
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
@@ -3951,7 +4001,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>47</v>
       </c>
@@ -3967,7 +4017,7 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D2" xr:uid="{5AF61348-CAED-40CF-A570-1ABFD106084D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="D2">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3985,23 +4035,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC31209-2B08-4392-B497-DB73B87283ED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="14" width="6.7109375" customWidth="1"/>
-    <col min="15" max="15" width="4.28515625" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" customWidth="1"/>
+    <col min="2" max="2" width="10.26953125" customWidth="1"/>
+    <col min="3" max="14" width="6.7265625" customWidth="1"/>
+    <col min="15" max="15" width="4.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>54</v>
       </c>
@@ -4023,8 +4073,8 @@
       <c r="Q1" s="27"/>
       <c r="R1" s="27"/>
     </row>
-    <row r="2" spans="1:18" ht="255.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:18" ht="162.4" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:18" ht="255.75" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:18" ht="162.4" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <conditionalFormatting sqref="C2:O2">
     <cfRule type="expression" dxfId="13" priority="4">
@@ -4051,7 +4101,7 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>38100</xdr:colOff>
                     <xdr:row>0</xdr:row>
-                    <xdr:rowOff>85725</xdr:rowOff>
+                    <xdr:rowOff>88900</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>17</xdr:col>
@@ -4071,7 +4121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A9704F8-A182-4E46-AA8E-61DC7E255DF6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -4079,20 +4129,20 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="2.7265625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="50.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="21.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.7265625" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="50.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" customWidth="1"/>
     <col min="9" max="9" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="50.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="15" t="s">
         <v>18</v>
       </c>
@@ -4100,19 +4150,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>51</v>
       </c>
       <c r="B2" s="4" t="str">
         <f ca="1">IF(TODAY()&gt;=MIN(DynamicTaskData[Start date]),"Today","")</f>
-        <v>Today</v>
+        <v/>
       </c>
       <c r="C2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>52</v>
       </c>
@@ -4123,30 +4173,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <f ca="1">IFERROR(IF(TODAY()&lt;MIN(DynamicTaskData[Start date]),MIN($B$11,MIN(DynamicTaskData[Start date])),TODAY()),TODAY())</f>
-        <v>43388</v>
+        <v>43397</v>
       </c>
       <c r="C4" s="3">
         <f ca="1">IFERROR(IF(Track_Today="Yes",IF(TODAY()&lt;MIN(DynamicTaskData[Start date]),0,9),0),0)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <f ca="1">IFERROR(IF(TODAY()&lt;MIN(DynamicTaskData[Start date]),MIN($B$11,MIN(DynamicTaskData[Start date])),TODAY()),TODAY())</f>
-        <v>43388</v>
+        <v>43397</v>
       </c>
       <c r="C5" s="3">
         <f ca="1">IFERROR(IF(Track_Today="Yes",IF(TODAY()&lt;MIN(DynamicTaskData[Start date]),0,9),0),0)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
         <v>53</v>
       </c>
@@ -4154,15 +4204,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B8" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="15" t="s">
         <v>64</v>
       </c>
@@ -4173,22 +4223,22 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <f ca="1">IFERROR(IF(ScrollingIncrement[scroll increment]=0,Start_Date,IF(Start_Date+ScrollingIncrement[scroll increment]*15&lt;End_Date,Start_Date+ScrollingIncrement[scroll increment]*15,End_Date-1)),"")</f>
-        <v>43387</v>
+        <v>43432</v>
       </c>
       <c r="D11">
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B12" s="2">
         <f ca="1">IFERROR(IF($B$11+15&lt;End_Date,$B$11+15,End_Date),"")</f>
-        <v>43402</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>43440</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>57</v>
       </c>
@@ -4208,36 +4258,36 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Chart Data'!$H6,ScrollingIncrement[scroll increment],0,1,1))=0,"",IF(OR(OFFSET('Chart Data'!$I6,ScrollingIncrement[scroll increment],0,1,1)&lt;=$B$12,OFFSET('Chart Data'!$H6,ScrollingIncrement[scroll increment],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tasks[],OFFSET('Chart Data'!$G6,ScrollingIncrement[scroll increment],0,1,1),4),"")),"")</f>
-        <v>Edit and Review SRS</v>
+        <v>Create TDD</v>
       </c>
       <c r="C15" s="25">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,$B$11,INDEX(Tasks[],OFFSET('Chart Data'!$G6,ScrollingIncrement[scroll increment],0,1,1),2)),"")</f>
-        <v>43387</v>
+        <v>43397</v>
       </c>
       <c r="D15" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,0,IF(AND('Chart Data'!$H6&lt;=$B$12,'Chart Data'!$I6&gt;=$B$12),ABS(OFFSET('Chart Data'!$H6,ScrollingIncrement[scroll increment],0,1,1)-$B$12)+1,OFFSET('Chart Data'!$K6,ScrollingIncrement[scroll increment],0,1,1))),"")</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E15">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,"",8),"")</f>
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Chart Data'!$H7,ScrollingIncrement[scroll increment],0,1,1))=0,"",IF(OR(OFFSET('Chart Data'!$I7,ScrollingIncrement[scroll increment],0,1,1)&lt;=$B$12,OFFSET('Chart Data'!$H7,ScrollingIncrement[scroll increment],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tasks[],OFFSET('Chart Data'!$G7,ScrollingIncrement[scroll increment],0,1,1),4),"")),"")</f>
-        <v>Create Vision Document</v>
+        <v>Character Movement</v>
       </c>
       <c r="C16" s="25">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,$B$11,INDEX(Tasks[],OFFSET('Chart Data'!$G7,ScrollingIncrement[scroll increment],0,1,1),2)),"")</f>
-        <v>43388</v>
+        <v>43400</v>
       </c>
       <c r="D16" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,0,IF(AND('Chart Data'!$H7&lt;=$B$12,'Chart Data'!$I7&gt;=$B$12),ABS(OFFSET('Chart Data'!$H7,ScrollingIncrement[scroll increment],0,1,1)-$B$12)+1,OFFSET('Chart Data'!$K7,ScrollingIncrement[scroll increment],0,1,1))),"")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E16" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,"",7),"")</f>
@@ -4247,21 +4297,21 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>63</v>
       </c>
       <c r="B17" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Chart Data'!$H8,ScrollingIncrement[scroll increment],0,1,1))=0,"",IF(OR(OFFSET('Chart Data'!$I8,ScrollingIncrement[scroll increment],0,1,1)&lt;=$B$12,OFFSET('Chart Data'!$H8,ScrollingIncrement[scroll increment],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tasks[],OFFSET('Chart Data'!$G8,ScrollingIncrement[scroll increment],0,1,1),4),"")),"")</f>
-        <v>Create GDD</v>
+        <v>Create a modular item system</v>
       </c>
       <c r="C17" s="25">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,$B$11,INDEX(Tasks[],OFFSET('Chart Data'!$G8,ScrollingIncrement[scroll increment],0,1,1),2)),"")</f>
-        <v>43390</v>
+        <v>43406</v>
       </c>
       <c r="D17" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,0,IF(AND('Chart Data'!$H8&lt;=$B$12,'Chart Data'!$I8&gt;=$B$12),ABS(OFFSET('Chart Data'!$H8,ScrollingIncrement[scroll increment],0,1,1)-$B$12)+1,OFFSET('Chart Data'!$K8,ScrollingIncrement[scroll increment],0,1,1))),"")</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E17" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,"",6),"")</f>
@@ -4280,18 +4330,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Chart Data'!$H9,ScrollingIncrement[scroll increment],0,1,1))=0,"",IF(OR(OFFSET('Chart Data'!$I9,ScrollingIncrement[scroll increment],0,1,1)&lt;=$B$12,OFFSET('Chart Data'!$H9,ScrollingIncrement[scroll increment],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tasks[],OFFSET('Chart Data'!$G9,ScrollingIncrement[scroll increment],0,1,1),4),"")),"")</f>
-        <v>Create TDD</v>
+        <v>Create modular item interactions</v>
       </c>
       <c r="C18" s="25">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,$B$11,INDEX(Tasks[],OFFSET('Chart Data'!$G9,ScrollingIncrement[scroll increment],0,1,1),2)),"")</f>
-        <v>43397</v>
+        <v>43413</v>
       </c>
       <c r="D18" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,0,IF(AND('Chart Data'!$H9&lt;=$B$12,'Chart Data'!$I9&gt;=$B$12),ABS(OFFSET('Chart Data'!$H9,ScrollingIncrement[scroll increment],0,1,1)-$B$12)+1,OFFSET('Chart Data'!$K9,ScrollingIncrement[scroll increment],0,1,1))),"")</f>
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E18" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,"",5),"")</f>
@@ -4310,14 +4360,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Chart Data'!$H10,ScrollingIncrement[scroll increment],0,1,1))=0,"",IF(OR(OFFSET('Chart Data'!$I10,ScrollingIncrement[scroll increment],0,1,1)&lt;=$B$12,OFFSET('Chart Data'!$H10,ScrollingIncrement[scroll increment],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tasks[],OFFSET('Chart Data'!$G10,ScrollingIncrement[scroll increment],0,1,1),4),"")),"")</f>
-        <v>Character can move</v>
+        <v>Create inventory item and in-world item</v>
       </c>
       <c r="C19" s="25">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,$B$11,INDEX(Tasks[],OFFSET('Chart Data'!$G10,ScrollingIncrement[scroll increment],0,1,1),2)),"")</f>
-        <v>43400</v>
+        <v>43430</v>
       </c>
       <c r="D19" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,0,IF(AND('Chart Data'!$H10&lt;=$B$12,'Chart Data'!$I10&gt;=$B$12),ABS(OFFSET('Chart Data'!$H10,ScrollingIncrement[scroll increment],0,1,1)-$B$12)+1,OFFSET('Chart Data'!$K10,ScrollingIncrement[scroll increment],0,1,1))),"")</f>
@@ -4340,18 +4390,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Chart Data'!$H11,ScrollingIncrement[scroll increment],0,1,1))=0,"",IF(OR(OFFSET('Chart Data'!$I11,ScrollingIncrement[scroll increment],0,1,1)&lt;=$B$12,OFFSET('Chart Data'!$H11,ScrollingIncrement[scroll increment],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tasks[],OFFSET('Chart Data'!$G11,ScrollingIncrement[scroll increment],0,1,1),4),"")),"")</f>
-        <v>Create a modular item system</v>
+        <v>Bug Fixes</v>
       </c>
       <c r="C20" s="25">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,$B$11,INDEX(Tasks[],OFFSET('Chart Data'!$G11,ScrollingIncrement[scroll increment],0,1,1),2)),"")</f>
-        <v>43406</v>
+        <v>43432</v>
       </c>
       <c r="D20" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,0,IF(AND('Chart Data'!$H11&lt;=$B$12,'Chart Data'!$I11&gt;=$B$12),ABS(OFFSET('Chart Data'!$H11,ScrollingIncrement[scroll increment],0,1,1)-$B$12)+1,OFFSET('Chart Data'!$K11,ScrollingIncrement[scroll increment],0,1,1))),"")</f>
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E20" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,"",3),"")</f>
@@ -4367,180 +4417,180 @@
       </c>
       <c r="I20" s="8">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C8),"")</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Chart Data'!$H12,ScrollingIncrement[scroll increment],0,1,1))=0,"",IF(OR(OFFSET('Chart Data'!$I12,ScrollingIncrement[scroll increment],0,1,1)&lt;=$B$12,OFFSET('Chart Data'!$H12,ScrollingIncrement[scroll increment],0,1,1)&gt;=($B$11-$D$11)),INDEX(Tasks[],OFFSET('Chart Data'!$G12,ScrollingIncrement[scroll increment],0,1,1),4),"")),"")</f>
-        <v>Create modular item interactions</v>
+        <v/>
       </c>
       <c r="C21" s="25">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,$B$11,INDEX(Tasks[],OFFSET('Chart Data'!$G12,ScrollingIncrement[scroll increment],0,1,1),2)),"")</f>
-        <v>43413</v>
+        <v>43432</v>
       </c>
       <c r="D21" s="3">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,0,IF(AND('Chart Data'!$H12&lt;=$B$12,'Chart Data'!$I12&gt;=$B$12),ABS(OFFSET('Chart Data'!$H12,ScrollingIncrement[scroll increment],0,1,1)-$B$12)+1,OFFSET('Chart Data'!$K12,ScrollingIncrement[scroll increment],0,1,1))),"")</f>
-        <v>15</v>
-      </c>
-      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3" t="str">
         <f ca="1">IFERROR(IF(LEN(DynamicTaskData[[#This Row],[Tasks]])=0,"",2),"")</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="G21" s="7" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!D9)=0,"",IF(AND('Chart Data'!D9&lt;=$B$12,'Chart Data'!D9&gt;=$B$11-$D$11),'Chart Data'!E9,"")),"")</f>
-        <v/>
+        <v>TDD</v>
       </c>
       <c r="H21" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D9),2)</f>
-        <v>43402</v>
-      </c>
-      <c r="I21" s="8" t="str">
+        <v>43404</v>
+      </c>
+      <c r="I21" s="8">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C9),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G22" s="7" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!D10)=0,"",IF(AND('Chart Data'!D10&lt;=$B$12,'Chart Data'!D10&gt;=$B$11-$D$11),'Chart Data'!E10,"")),"")</f>
-        <v/>
+        <v>Movement</v>
       </c>
       <c r="H22" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D10),2)</f>
-        <v>43402</v>
-      </c>
-      <c r="I22" s="8" t="str">
+        <v>43407</v>
+      </c>
+      <c r="I22" s="8">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C10),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G23" s="7" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!D11)=0,"",IF(AND('Chart Data'!D11&lt;=$B$12,'Chart Data'!D11&gt;=$B$11-$D$11),'Chart Data'!E11,"")),"")</f>
-        <v/>
+        <v>Item System</v>
       </c>
       <c r="H23" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D11),2)</f>
-        <v>43402</v>
-      </c>
-      <c r="I23" s="8" t="str">
+        <v>43427</v>
+      </c>
+      <c r="I23" s="8">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C11),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G24" s="7" t="str">
         <f ca="1">IFERROR(IF(LEN('Chart Data'!D12)=0,"",IF(AND('Chart Data'!D12&lt;=$B$12,'Chart Data'!D12&gt;=$B$11-$D$11),'Chart Data'!E12,"")),"")</f>
-        <v/>
+        <v>MVP</v>
       </c>
       <c r="H24" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D12),2)</f>
-        <v>43402</v>
-      </c>
-      <c r="I24" s="8" t="str">
+        <v>43440</v>
+      </c>
+      <c r="I24" s="8">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C12),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G25" s="7" t="str">
         <f>IFERROR(IF(LEN('Chart Data'!D13)=0,"",IF(AND('Chart Data'!D13&lt;=$B$12,'Chart Data'!D13&gt;=$B$11-$D$11),'Chart Data'!E13,"")),"")</f>
         <v/>
       </c>
       <c r="H25" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D13),2)</f>
-        <v>43402</v>
+        <v>43440</v>
       </c>
       <c r="I25" s="8" t="str">
         <f>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C13),"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G26" s="7" t="str">
         <f>IFERROR(IF(LEN('Chart Data'!D14)=0,"",IF(AND('Chart Data'!D14&lt;=$B$12,'Chart Data'!D14&gt;=$B$11-$D$11),'Chart Data'!E14,"")),"")</f>
         <v/>
       </c>
       <c r="H26" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D14),2)</f>
-        <v>43402</v>
+        <v>43440</v>
       </c>
       <c r="I26" s="8" t="str">
         <f>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C14),"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G27" s="7" t="str">
         <f>IFERROR(IF(LEN('Chart Data'!D15)=0,"",IF(AND('Chart Data'!D15&lt;=$B$12,'Chart Data'!D15&gt;=$B$11-$D$11),'Chart Data'!E15,"")),"")</f>
         <v/>
       </c>
       <c r="H27" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D15),2)</f>
-        <v>43402</v>
+        <v>43440</v>
       </c>
       <c r="I27" s="8" t="str">
         <f>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C15),"")</f>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G28" s="7" t="str">
         <f>IFERROR(IF(LEN('Chart Data'!D16)=0,"",IF(AND('Chart Data'!D16&lt;=$B$12,'Chart Data'!D16&gt;=$B$11-$D$11),'Chart Data'!E16,"")),"")</f>
         <v/>
       </c>
       <c r="H28" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D16),2)</f>
-        <v>43402</v>
+        <v>43440</v>
       </c>
       <c r="I28" s="8" t="str">
         <f>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C16),"")</f>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G29" s="7" t="str">
         <f>IFERROR(IF(LEN('Chart Data'!D17)=0,"",IF(AND('Chart Data'!D17&lt;=$B$12,'Chart Data'!D17&gt;=$B$11-$D$11),'Chart Data'!E17,"")),"")</f>
         <v/>
       </c>
       <c r="H29" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D17),2)</f>
-        <v>43402</v>
+        <v>43440</v>
       </c>
       <c r="I29" s="8" t="str">
         <f>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C17),"")</f>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G30" s="7" t="str">
         <f>IFERROR(IF(LEN('Chart Data'!D18)=0,"",IF(AND('Chart Data'!D18&lt;=$B$12,'Chart Data'!D18&gt;=$B$11-$D$11),'Chart Data'!E18,"")),"")</f>
         <v/>
       </c>
       <c r="H30" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D18),2)</f>
-        <v>43402</v>
+        <v>43440</v>
       </c>
       <c r="I30" s="8" t="str">
         <f>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C18),"")</f>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G31" s="7" t="str">
         <f>IFERROR(IF(LEN('Chart Data'!D19)=0,"",IF(AND('Chart Data'!D19&lt;=$B$12,'Chart Data'!D19&gt;=$B$11-$D$11),'Chart Data'!E19,"")),"")</f>
         <v/>
       </c>
       <c r="H31" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D19),2)</f>
-        <v>43402</v>
+        <v>43440</v>
       </c>
       <c r="I31" s="8" t="str">
         <f>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C19),"")</f>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>62</v>
       </c>
@@ -4550,7 +4600,7 @@
       </c>
       <c r="H32" s="22">
         <f ca="1">IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,$B$12,'Chart Data'!$D20),2)</f>
-        <v>43402</v>
+        <v>43440</v>
       </c>
       <c r="I32" s="8" t="str">
         <f>IFERROR(IF(LEN(DynamicMilestoneData[[#This Row],[Milestones]])=0,"",'Chart Data'!$C20),"")</f>
@@ -4582,69 +4632,69 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2D9CFDD-EC4B-4303-9E14-A49D2BBA1837}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="78.7109375" customWidth="1"/>
+    <col min="1" max="1" width="78.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="50.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="150" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="255" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="180" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="174" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="58" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>